<commit_message>
Initial check-in of kinetics data factsheet
</commit_message>
<xml_diff>
--- a/models/pinocembrin_kinetics.xlsx
+++ b/models/pinocembrin_kinetics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="P35510" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -613,7 +613,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B3" sqref="B3:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -650,212 +650,278 @@
       </c>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3">
+      <c r="B3" s="2">
         <v>6.1000000000000004E-3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4">
+      <c r="B4" s="2">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1.8800000000000001E-2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>2.9000000000000001E-2</v>
       </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6">
+      <c r="B6" s="2">
         <v>2.1299999999999999E-2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>2.1700000000000001E-2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>3.5999999999999997E-2</v>
       </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7">
+      <c r="B7" s="2">
         <v>0.182</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>2.3E-2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>6.5000000000000002E-2</v>
       </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8">
+      <c r="B8" s="2">
         <v>0.26</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>2.8199999999999999E-2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0.151</v>
       </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0.3</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0.16300000000000001</v>
       </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10">
+      <c r="B10" s="2">
         <v>0.37</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0.17</v>
       </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="C11">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2">
         <v>0.05</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0.17299999999999999</v>
       </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="C12">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2">
         <v>5.4399999999999997E-2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>0.24</v>
       </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="C13">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>1.5069999999999999</v>
       </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:5">
-      <c r="C14">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="C15">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2">
         <v>6.6000000000000003E-2</v>
       </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="C16">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2">
         <v>0.26</v>
       </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="C17">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2">
         <v>0.28000000000000003</v>
       </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="C18">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2">
         <v>0.29199999999999998</v>
       </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="C19">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2">
         <v>1.048</v>
       </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="C20">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2">
         <v>1.1000000000000001</v>
       </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="C21">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2">
         <v>1.1000000000000001</v>
       </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="C22">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2">
         <v>1.3</v>
       </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="C23">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2">
         <v>1.7</v>
       </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="C24">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2">
         <v>1.7</v>
       </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="C25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2">
         <v>2.0699999999999998</v>
       </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="C26">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2">
         <v>4.4000000000000004</v>
       </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="C27">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2">
         <v>4.4000000000000004</v>
       </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="C28">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2">
         <v>4.5</v>
       </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="C29">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2">
         <v>6.32</v>
       </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="C30">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2">
         <v>6.35</v>
       </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="C31">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2">
         <v>6.63</v>
       </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
@@ -914,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1177,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1203,73 +1269,76 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="B3">
+      <c r="B3" s="2">
         <v>51.3</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>7.1999999999999998E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4">
+      <c r="B4" s="2">
         <v>84.5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5">
+      <c r="B5" s="2">
         <v>107</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.01</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="B6">
+      <c r="B6" s="2">
         <v>167</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="B7">
+      <c r="B7" s="2">
         <v>183</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0.02</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="B8">
+      <c r="B8" s="2">
         <v>32.5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0.03</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="B9">
+      <c r="B9" s="2">
         <v>62.5</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>0.12</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="C10">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2">
         <v>0.18</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="C11">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="C12">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>

</xml_diff>